<commit_message>
Updated chapter 1 with sound
</commit_message>
<xml_diff>
--- a/materialer/indholdsfortegnelse.xlsx
+++ b/materialer/indholdsfortegnelse.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tlinnet/software/hoer-laegedansk/materialer/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6459C67-8832-A641-AAAC-896998E13D29}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9312F872-8B9F-D24D-A2BD-92AE96460460}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15540" firstSheet="2" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3728" uniqueCount="2344">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3747" uniqueCount="2344">
   <si>
     <t>Mødet mellem læge og patient</t>
   </si>
@@ -30702,7 +30702,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E5E8D912-FB3D-A540-9B81-CC99B84FAB3E}">
   <dimension ref="A1:C217"/>
   <sheetViews>
-    <sheetView topLeftCell="A198" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
@@ -33754,9 +33754,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03E3B2D6-1357-EF4F-B237-AF77DB97A715}">
   <dimension ref="A1:P460"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="N5" sqref="N5"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A215" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="L8" sqref="L8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -33768,7 +33768,7 @@
     <col min="5" max="5" width="9.6640625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="9.1640625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="6.6640625" style="11" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="4.5" style="11" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="5.6640625" style="11" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="3.5" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="3.1640625" customWidth="1"/>
     <col min="11" max="11" width="8.6640625" style="8" bestFit="1" customWidth="1"/>
@@ -33915,21 +33915,27 @@
         <v>211</v>
       </c>
       <c r="D5" t="s">
-        <v>190</v>
+        <v>204</v>
       </c>
       <c r="E5" t="s">
         <v>210</v>
       </c>
+      <c r="G5" s="8">
+        <v>3</v>
+      </c>
+      <c r="H5" s="8">
+        <v>32</v>
+      </c>
       <c r="K5" s="8">
-        <v>1</v>
-      </c>
-      <c r="L5" s="7">
+        <v>32</v>
+      </c>
+      <c r="L5" s="7" t="str">
         <f>VLOOKUP(K5,Side_til_Sektion!A$2:C$217,3,FALSE)</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="P5" t="str">
         <f t="shared" si="0"/>
-        <v>| OP-JOUR || Forord ||  ||  || 1 || 0 || &lt;html5media&gt;File:OP-JOUR.mp3&lt;/html5media&gt;</v>
+        <v>| OP-JOUR || Kapitel || 3 ||  || 32 || 3 || &lt;html5media&gt;File:OP-JOUR.mp3&lt;/html5media&gt;</v>
       </c>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.2">
@@ -33964,6 +33970,9 @@
         <f>VLOOKUP(K6,Side_til_Sektion!A$2:C$217,3,FALSE)</f>
         <v>1</v>
       </c>
+      <c r="N6" t="s">
+        <v>2343</v>
+      </c>
       <c r="P6" t="str">
         <f t="shared" si="0"/>
         <v>| KAP1_15 || Kapitel || 1 ||  || 15 || 1 || &lt;html5media&gt;File:KAP1_15.mp3&lt;/html5media&gt;</v>
@@ -34004,6 +34013,9 @@
         <f>VLOOKUP(K7,Side_til_Sektion!A$2:C$217,3,FALSE)</f>
         <v>1</v>
       </c>
+      <c r="N7" t="s">
+        <v>2343</v>
+      </c>
       <c r="P7" t="str">
         <f t="shared" si="0"/>
         <v>| KAP1_15_2 || Kapitel || 1 || 2 || 15 || 1 || &lt;html5media&gt;File:KAP1_15_2.mp3&lt;/html5media&gt;</v>
@@ -34041,6 +34053,9 @@
         <f>VLOOKUP(K8,Side_til_Sektion!A$2:C$217,3,FALSE)</f>
         <v>1.2</v>
       </c>
+      <c r="N8" t="s">
+        <v>2343</v>
+      </c>
       <c r="P8" t="str">
         <f t="shared" si="0"/>
         <v>| KAP1_16 || Kapitel || 1 ||  || 16 || 1.2 || &lt;html5media&gt;File:KAP1_16.mp3&lt;/html5media&gt;</v>
@@ -34081,6 +34096,9 @@
         <f>VLOOKUP(K9,Side_til_Sektion!A$2:C$217,3,FALSE)</f>
         <v>1.2</v>
       </c>
+      <c r="N9" t="s">
+        <v>2343</v>
+      </c>
       <c r="P9" t="str">
         <f t="shared" si="0"/>
         <v>| KAP1_16_2 || Kapitel || 1 || 2 || 16 || 1.2 || &lt;html5media&gt;File:KAP1_16_2.mp3&lt;/html5media&gt;</v>
@@ -34118,6 +34136,9 @@
         <f>VLOOKUP(K10,Side_til_Sektion!A$2:C$217,3,FALSE)</f>
         <v>1.2.2</v>
       </c>
+      <c r="N10" t="s">
+        <v>2343</v>
+      </c>
       <c r="P10" t="str">
         <f t="shared" si="0"/>
         <v>| KAP1_17 || Kapitel || 1 ||  || 17 || 1.2.2 || &lt;html5media&gt;File:KAP1_17.mp3&lt;/html5media&gt;</v>
@@ -34155,6 +34176,9 @@
         <f>VLOOKUP(K11,Side_til_Sektion!A$2:C$217,3,FALSE)</f>
         <v>1.2.3</v>
       </c>
+      <c r="N11" t="s">
+        <v>2343</v>
+      </c>
       <c r="P11" t="str">
         <f t="shared" si="0"/>
         <v>| KAP1_18 || Kapitel || 1 ||  || 18 || 1.2.3 || &lt;html5media&gt;File:KAP1_18.mp3&lt;/html5media&gt;</v>
@@ -34192,6 +34216,9 @@
         <f>VLOOKUP(K12,Side_til_Sektion!A$2:C$217,3,FALSE)</f>
         <v>1.3</v>
       </c>
+      <c r="N12" t="s">
+        <v>2343</v>
+      </c>
       <c r="P12" t="str">
         <f t="shared" si="0"/>
         <v>| KAP1_19 || Kapitel || 1 ||  || 19 || 1.3 || &lt;html5media&gt;File:KAP1_19.mp3&lt;/html5media&gt;</v>
@@ -34232,6 +34259,9 @@
         <f>VLOOKUP(K13,Side_til_Sektion!A$2:C$217,3,FALSE)</f>
         <v>1.3</v>
       </c>
+      <c r="N13" t="s">
+        <v>2343</v>
+      </c>
       <c r="P13" t="str">
         <f t="shared" si="0"/>
         <v>| KAP1_19_2 || Kapitel || 1 || 2 || 19 || 1.3 || &lt;html5media&gt;File:KAP1_19_2.mp3&lt;/html5media&gt;</v>
@@ -34272,6 +34302,9 @@
         <f>VLOOKUP(K14,Side_til_Sektion!A$2:C$217,3,FALSE)</f>
         <v>1.3</v>
       </c>
+      <c r="N14" t="s">
+        <v>2343</v>
+      </c>
       <c r="P14" t="str">
         <f t="shared" si="0"/>
         <v>| KAP1_19_3 || Kapitel || 1 || 3 || 19 || 1.3 || &lt;html5media&gt;File:KAP1_19_3.mp3&lt;/html5media&gt;</v>
@@ -34309,6 +34342,9 @@
         <f>VLOOKUP(K15,Side_til_Sektion!A$2:C$217,3,FALSE)</f>
         <v>1.3.3</v>
       </c>
+      <c r="N15" t="s">
+        <v>2343</v>
+      </c>
       <c r="P15" t="str">
         <f t="shared" si="0"/>
         <v>| KAP1_21 || Kapitel || 1 ||  || 21 || 1.3.3 || &lt;html5media&gt;File:KAP1_21.mp3&lt;/html5media&gt;</v>
@@ -34346,6 +34382,9 @@
         <f>VLOOKUP(K16,Side_til_Sektion!A$2:C$217,3,FALSE)</f>
         <v>1.3.4</v>
       </c>
+      <c r="N16" t="s">
+        <v>2343</v>
+      </c>
       <c r="P16" t="str">
         <f t="shared" si="0"/>
         <v>| KAP1_22 || Kapitel || 1 ||  || 22 || 1.3.4 || &lt;html5media&gt;File:KAP1_22.mp3&lt;/html5media&gt;</v>
@@ -34386,6 +34425,9 @@
         <f>VLOOKUP(K17,Side_til_Sektion!A$2:C$217,3,FALSE)</f>
         <v>1.3.4</v>
       </c>
+      <c r="N17" t="s">
+        <v>2343</v>
+      </c>
       <c r="P17" t="str">
         <f t="shared" si="0"/>
         <v>| KAP1_22_2 || Kapitel || 1 || 2 || 22 || 1.3.4 || &lt;html5media&gt;File:KAP1_22_2.mp3&lt;/html5media&gt;</v>
@@ -34426,6 +34468,9 @@
         <f>VLOOKUP(K18,Side_til_Sektion!A$2:C$217,3,FALSE)</f>
         <v>1.3.4</v>
       </c>
+      <c r="N18" t="s">
+        <v>2343</v>
+      </c>
       <c r="P18" t="str">
         <f t="shared" si="0"/>
         <v>| KAP1_22_3 || Kapitel || 1 || 3 || 22 || 1.3.4 || &lt;html5media&gt;File:KAP1_22_3.mp3&lt;/html5media&gt;</v>
@@ -34463,6 +34508,9 @@
         <f>VLOOKUP(K19,Side_til_Sektion!A$2:C$217,3,FALSE)</f>
         <v>1.4</v>
       </c>
+      <c r="N19" t="s">
+        <v>2343</v>
+      </c>
       <c r="P19" t="str">
         <f t="shared" si="0"/>
         <v>| KAP1_23 || Kapitel || 1 ||  || 23 || 1.4 || &lt;html5media&gt;File:KAP1_23.mp3&lt;/html5media&gt;</v>
@@ -42393,6 +42441,9 @@
         <f>VLOOKUP(K227,Side_til_Sektion!A$2:C$217,3,FALSE)</f>
         <v>1.3.3</v>
       </c>
+      <c r="N227" t="s">
+        <v>2343</v>
+      </c>
       <c r="P227" t="str">
         <f t="shared" si="3"/>
         <v>| BOKS21 || Bokse ||  ||  || 21 || 1.3.3 || &lt;html5media&gt;File:BOKS21.mp3&lt;/html5media&gt;</v>
@@ -42430,6 +42481,9 @@
         <f>VLOOKUP(K228,Side_til_Sektion!A$2:C$217,3,FALSE)</f>
         <v>1.3.3</v>
       </c>
+      <c r="N228" t="s">
+        <v>2343</v>
+      </c>
       <c r="P228" t="str">
         <f t="shared" si="3"/>
         <v>| BOKS21B || Bokse ||  || B || 21 || 1.3.3 || &lt;html5media&gt;File:BOKS21B.mp3&lt;/html5media&gt;</v>
@@ -42464,6 +42518,9 @@
         <f>VLOOKUP(K229,Side_til_Sektion!A$2:C$217,3,FALSE)</f>
         <v>1.4</v>
       </c>
+      <c r="N229" t="s">
+        <v>2343</v>
+      </c>
       <c r="P229" t="str">
         <f t="shared" si="3"/>
         <v>| BOKS23 || Bokse ||  ||  || 23 || 1.4 || &lt;html5media&gt;File:BOKS23.mp3&lt;/html5media&gt;</v>
@@ -42498,6 +42555,9 @@
         <f>VLOOKUP(K230,Side_til_Sektion!A$2:C$217,3,FALSE)</f>
         <v>1.4</v>
       </c>
+      <c r="N230" t="s">
+        <v>2343</v>
+      </c>
       <c r="P230" t="str">
         <f t="shared" si="3"/>
         <v>| BOKS24 || Bokse ||  ||  || 24 || 1.4 || &lt;html5media&gt;File:BOKS24.mp3&lt;/html5media&gt;</v>
@@ -42534,6 +42594,9 @@
       <c r="L231" s="7" t="str">
         <f>VLOOKUP(K231,Side_til_Sektion!A$2:C$217,3,FALSE)</f>
         <v>1.4</v>
+      </c>
+      <c r="N231" t="s">
+        <v>2343</v>
       </c>
       <c r="P231" t="str">
         <f t="shared" si="3"/>

</xml_diff>

<commit_message>
Added sound to chapter 2
</commit_message>
<xml_diff>
--- a/materialer/indholdsfortegnelse.xlsx
+++ b/materialer/indholdsfortegnelse.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tlinnet/software/hoer-laegedansk/materialer/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9312F872-8B9F-D24D-A2BD-92AE96460460}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71B2D211-C340-6940-8536-FE38A8618E84}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15540" firstSheet="2" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3747" uniqueCount="2344">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3753" uniqueCount="2344">
   <si>
     <t>Mødet mellem læge og patient</t>
   </si>
@@ -33754,9 +33754,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03E3B2D6-1357-EF4F-B237-AF77DB97A715}">
   <dimension ref="A1:P460"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A215" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L8" sqref="L8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A217" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="N233" sqref="N233"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -34548,6 +34548,9 @@
         <f>VLOOKUP(K20,Side_til_Sektion!A$2:C$217,3,FALSE)</f>
         <v>2</v>
       </c>
+      <c r="N20" t="s">
+        <v>2343</v>
+      </c>
       <c r="P20" t="str">
         <f t="shared" si="0"/>
         <v>| KAP2_25 || Kapitel || 2 ||  || 25 || 2 || &lt;html5media&gt;File:KAP2_25.mp3&lt;/html5media&gt;</v>
@@ -34588,6 +34591,9 @@
         <f>VLOOKUP(K21,Side_til_Sektion!A$2:C$217,3,FALSE)</f>
         <v>2</v>
       </c>
+      <c r="N21" t="s">
+        <v>2343</v>
+      </c>
       <c r="P21" t="str">
         <f t="shared" si="0"/>
         <v>| KAP2_25_2 || Kapitel || 2 || 2 || 25 || 2 || &lt;html5media&gt;File:KAP2_25_2.mp3&lt;/html5media&gt;</v>
@@ -34625,6 +34631,9 @@
         <f>VLOOKUP(K22,Side_til_Sektion!A$2:C$217,3,FALSE)</f>
         <v>2.3</v>
       </c>
+      <c r="N22" t="s">
+        <v>2343</v>
+      </c>
       <c r="P22" t="str">
         <f t="shared" si="0"/>
         <v>| KAP2_27 || Kapitel || 2 ||  || 27 || 2.3 || &lt;html5media&gt;File:KAP2_27.mp3&lt;/html5media&gt;</v>
@@ -34665,6 +34674,9 @@
         <f>VLOOKUP(K23,Side_til_Sektion!A$2:C$217,3,FALSE)</f>
         <v>2.3</v>
       </c>
+      <c r="N23" t="s">
+        <v>2343</v>
+      </c>
       <c r="P23" t="str">
         <f t="shared" si="0"/>
         <v>| KAP2_27_2 || Kapitel || 2 || 2 || 27 || 2.3 || &lt;html5media&gt;File:KAP2_27_2.mp3&lt;/html5media&gt;</v>
@@ -34702,6 +34714,9 @@
         <f>VLOOKUP(K24,Side_til_Sektion!A$2:C$217,3,FALSE)</f>
         <v>2.5</v>
       </c>
+      <c r="N24" t="s">
+        <v>2343</v>
+      </c>
       <c r="P24" t="str">
         <f t="shared" si="0"/>
         <v>| KAP2_29 || Kapitel || 2 ||  || 29 || 2.5 || &lt;html5media&gt;File:KAP2_29.mp3&lt;/html5media&gt;</v>
@@ -42631,6 +42646,9 @@
       <c r="L232" s="7" t="str">
         <f>VLOOKUP(K232,Side_til_Sektion!A$2:C$217,3,FALSE)</f>
         <v>2</v>
+      </c>
+      <c r="N232" t="s">
+        <v>2343</v>
       </c>
       <c r="P232" t="str">
         <f t="shared" si="3"/>

</xml_diff>

<commit_message>
Added sound to chapter 3
</commit_message>
<xml_diff>
--- a/materialer/indholdsfortegnelse.xlsx
+++ b/materialer/indholdsfortegnelse.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tlinnet/software/hoer-laegedansk/materialer/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71B2D211-C340-6940-8536-FE38A8618E84}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCB24FAD-F8FD-254E-B9FF-CFCCB15870A4}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15540" firstSheet="2" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3753" uniqueCount="2344">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3796" uniqueCount="2344">
   <si>
     <t>Mødet mellem læge og patient</t>
   </si>
@@ -33755,8 +33755,8 @@
   <dimension ref="A1:P460"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A217" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="N233" sqref="N233"/>
+      <pane ySplit="1" topLeftCell="A43" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="N63" sqref="N63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -34754,6 +34754,9 @@
         <f>VLOOKUP(K25,Side_til_Sektion!A$2:C$217,3,FALSE)</f>
         <v>3</v>
       </c>
+      <c r="N25" t="s">
+        <v>2343</v>
+      </c>
       <c r="P25" t="str">
         <f t="shared" si="0"/>
         <v>| KAP3_31 || Kapitel || 3 ||  || 31 || 3 || &lt;html5media&gt;File:KAP3_31.mp3&lt;/html5media&gt;</v>
@@ -34794,6 +34797,9 @@
         <f>VLOOKUP(K26,Side_til_Sektion!A$2:C$217,3,FALSE)</f>
         <v>3</v>
       </c>
+      <c r="N26" t="s">
+        <v>2343</v>
+      </c>
       <c r="P26" t="str">
         <f t="shared" si="0"/>
         <v>| KAP3_31_2 || Kapitel || 3 || 2 || 31 || 3 || &lt;html5media&gt;File:KAP3_31_2.mp3&lt;/html5media&gt;</v>
@@ -34834,6 +34840,9 @@
         <f>VLOOKUP(K27,Side_til_Sektion!A$2:C$217,3,FALSE)</f>
         <v>3</v>
       </c>
+      <c r="N27" t="s">
+        <v>2343</v>
+      </c>
       <c r="P27" t="str">
         <f t="shared" si="0"/>
         <v>| KAP3_31_3 || Kapitel || 3 || 3 || 31 || 3 || &lt;html5media&gt;File:KAP3_31_3.mp3&lt;/html5media&gt;</v>
@@ -34871,6 +34880,9 @@
         <f>VLOOKUP(K28,Side_til_Sektion!A$2:C$217,3,FALSE)</f>
         <v>3.1.2</v>
       </c>
+      <c r="N28" t="s">
+        <v>2343</v>
+      </c>
       <c r="P28" t="str">
         <f t="shared" si="0"/>
         <v>| KAP3_33 || Kapitel || 3 ||  || 33 || 3.1.2 || &lt;html5media&gt;File:KAP3_33.mp3&lt;/html5media&gt;</v>
@@ -34911,6 +34923,9 @@
         <f>VLOOKUP(K29,Side_til_Sektion!A$2:C$217,3,FALSE)</f>
         <v>3.1.2</v>
       </c>
+      <c r="N29" t="s">
+        <v>2343</v>
+      </c>
       <c r="P29" t="str">
         <f t="shared" si="0"/>
         <v>| KAP3_33_2 || Kapitel || 3 || 2 || 33 || 3.1.2 || &lt;html5media&gt;File:KAP3_33_2.mp3&lt;/html5media&gt;</v>
@@ -34948,6 +34963,9 @@
         <f>VLOOKUP(K30,Side_til_Sektion!A$2:C$217,3,FALSE)</f>
         <v>3.1.4</v>
       </c>
+      <c r="N30" t="s">
+        <v>2343</v>
+      </c>
       <c r="P30" t="str">
         <f t="shared" si="0"/>
         <v>| KAP3_34 || Kapitel || 3 ||  || 34 || 3.1.4 || &lt;html5media&gt;File:KAP3_34.mp3&lt;/html5media&gt;</v>
@@ -34985,6 +35003,9 @@
         <f>VLOOKUP(K31,Side_til_Sektion!A$2:C$217,3,FALSE)</f>
         <v>3.1.5</v>
       </c>
+      <c r="N31" t="s">
+        <v>2343</v>
+      </c>
       <c r="P31" t="str">
         <f t="shared" si="0"/>
         <v>| KAP3_35 || Kapitel || 3 ||  || 35 || 3.1.5 || &lt;html5media&gt;File:KAP3_35.mp3&lt;/html5media&gt;</v>
@@ -35022,6 +35043,9 @@
         <f>VLOOKUP(K32,Side_til_Sektion!A$2:C$217,3,FALSE)</f>
         <v>3.1.6</v>
       </c>
+      <c r="N32" t="s">
+        <v>2343</v>
+      </c>
       <c r="P32" t="str">
         <f t="shared" si="0"/>
         <v>| KAP3_36 || Kapitel || 3 ||  || 36 || 3.1.6 || &lt;html5media&gt;File:KAP3_36.mp3&lt;/html5media&gt;</v>
@@ -35059,6 +35083,9 @@
         <f>VLOOKUP(K33,Side_til_Sektion!A$2:C$217,3,FALSE)</f>
         <v>3.1.7</v>
       </c>
+      <c r="N33" t="s">
+        <v>2343</v>
+      </c>
       <c r="P33" t="str">
         <f t="shared" si="0"/>
         <v>| kap3_37 || Kapitel || 3 ||  || 37 || 3.1.7 || &lt;html5media&gt;File:kap3_37.mp3&lt;/html5media&gt;</v>
@@ -35096,6 +35123,9 @@
         <f>VLOOKUP(K34,Side_til_Sektion!A$2:C$217,3,FALSE)</f>
         <v>3.1.8</v>
       </c>
+      <c r="N34" t="s">
+        <v>2343</v>
+      </c>
       <c r="P34" t="str">
         <f t="shared" si="0"/>
         <v>| KAP3_39 || Kapitel || 3 ||  || 39 || 3.1.8 || &lt;html5media&gt;File:KAP3_39.mp3&lt;/html5media&gt;</v>
@@ -35133,6 +35163,9 @@
         <f>VLOOKUP(K35,Side_til_Sektion!A$2:C$217,3,FALSE)</f>
         <v>3.1.9</v>
       </c>
+      <c r="N35" t="s">
+        <v>2343</v>
+      </c>
       <c r="P35" t="str">
         <f t="shared" si="0"/>
         <v>| KAP3_41 || Kapitel || 3 ||  || 41 || 3.1.9 || &lt;html5media&gt;File:KAP3_41.mp3&lt;/html5media&gt;</v>
@@ -35170,6 +35203,9 @@
         <f>VLOOKUP(K36,Side_til_Sektion!A$2:C$217,3,FALSE)</f>
         <v>3.1.10</v>
       </c>
+      <c r="N36" t="s">
+        <v>2343</v>
+      </c>
       <c r="P36" t="str">
         <f t="shared" si="0"/>
         <v>| KAP3_42 || Kapitel || 3 ||  || 42 || 3.1.10 || &lt;html5media&gt;File:KAP3_42.mp3&lt;/html5media&gt;</v>
@@ -35210,6 +35246,9 @@
         <f>VLOOKUP(K37,Side_til_Sektion!A$2:C$217,3,FALSE)</f>
         <v>3.1.10</v>
       </c>
+      <c r="N37" t="s">
+        <v>2343</v>
+      </c>
       <c r="P37" t="str">
         <f t="shared" si="0"/>
         <v>| KAP3_42_2 || Kapitel || 3 || 2 || 42 || 3.1.10 || &lt;html5media&gt;File:KAP3_42_2.mp3&lt;/html5media&gt;</v>
@@ -35247,6 +35286,9 @@
         <f>VLOOKUP(K38,Side_til_Sektion!A$2:C$217,3,FALSE)</f>
         <v>3.2</v>
       </c>
+      <c r="N38" t="s">
+        <v>2343</v>
+      </c>
       <c r="P38" t="str">
         <f t="shared" si="0"/>
         <v>| KAP3_43 || Kapitel || 3 ||  || 43 || 3.2 || &lt;html5media&gt;File:KAP3_43.mp3&lt;/html5media&gt;</v>
@@ -35284,6 +35326,9 @@
         <f>VLOOKUP(K39,Side_til_Sektion!A$2:C$217,3,FALSE)</f>
         <v>3.2.1</v>
       </c>
+      <c r="N39" t="s">
+        <v>2343</v>
+      </c>
       <c r="P39" t="str">
         <f t="shared" si="0"/>
         <v>| KAP3_44 || Kapitel || 3 ||  || 44 || 3.2.1 || &lt;html5media&gt;File:KAP3_44.mp3&lt;/html5media&gt;</v>
@@ -35321,6 +35366,9 @@
         <f>VLOOKUP(K40,Side_til_Sektion!A$2:C$217,3,FALSE)</f>
         <v>3.2.2</v>
       </c>
+      <c r="N40" t="s">
+        <v>2343</v>
+      </c>
       <c r="P40" t="str">
         <f t="shared" si="0"/>
         <v>| KAP3_45 || Kapitel || 3 ||  || 45 || 3.2.2 || &lt;html5media&gt;File:KAP3_45.mp3&lt;/html5media&gt;</v>
@@ -35361,6 +35409,9 @@
         <f>VLOOKUP(K41,Side_til_Sektion!A$2:C$217,3,FALSE)</f>
         <v>3.2.2</v>
       </c>
+      <c r="N41" t="s">
+        <v>2343</v>
+      </c>
       <c r="P41" t="str">
         <f t="shared" si="0"/>
         <v>| KAP3_45_2 || Kapitel || 3 || 2 || 45 || 3.2.2 || &lt;html5media&gt;File:KAP3_45_2.mp3&lt;/html5media&gt;</v>
@@ -35401,6 +35452,9 @@
         <f>VLOOKUP(K42,Side_til_Sektion!A$2:C$217,3,FALSE)</f>
         <v>3.2.2</v>
       </c>
+      <c r="N42" t="s">
+        <v>2343</v>
+      </c>
       <c r="P42" t="str">
         <f t="shared" si="0"/>
         <v>| KAP3_45_3 || Kapitel || 3 || 3 || 45 || 3.2.2 || &lt;html5media&gt;File:KAP3_45_3.mp3&lt;/html5media&gt;</v>
@@ -35438,6 +35492,9 @@
         <f>VLOOKUP(K43,Side_til_Sektion!A$2:C$217,3,FALSE)</f>
         <v>3.2.5</v>
       </c>
+      <c r="N43" t="s">
+        <v>2343</v>
+      </c>
       <c r="P43" t="str">
         <f t="shared" si="0"/>
         <v>| KAP3_46 || Kapitel || 3 ||  || 46 || 3.2.5 || &lt;html5media&gt;File:KAP3_46.mp3&lt;/html5media&gt;</v>
@@ -35478,6 +35535,9 @@
         <f>VLOOKUP(K44,Side_til_Sektion!A$2:C$217,3,FALSE)</f>
         <v>3.2.5</v>
       </c>
+      <c r="N44" t="s">
+        <v>2343</v>
+      </c>
       <c r="P44" t="str">
         <f t="shared" si="0"/>
         <v>| KAP3_46_2 || Kapitel || 3 || 2 || 46 || 3.2.5 || &lt;html5media&gt;File:KAP3_46_2.mp3&lt;/html5media&gt;</v>
@@ -35518,6 +35578,9 @@
         <f>VLOOKUP(K45,Side_til_Sektion!A$2:C$217,3,FALSE)</f>
         <v>3.2.5</v>
       </c>
+      <c r="N45" t="s">
+        <v>2343</v>
+      </c>
       <c r="P45" t="str">
         <f t="shared" si="0"/>
         <v>| KAP3_46_3 || Kapitel || 3 || 3 || 46 || 3.2.5 || &lt;html5media&gt;File:KAP3_46_3.mp3&lt;/html5media&gt;</v>
@@ -35558,6 +35621,9 @@
         <f>VLOOKUP(K46,Side_til_Sektion!A$2:C$217,3,FALSE)</f>
         <v>3.2.5</v>
       </c>
+      <c r="N46" t="s">
+        <v>2343</v>
+      </c>
       <c r="P46" t="str">
         <f t="shared" si="0"/>
         <v>| KAP3_46_4 || Kapitel || 3 || 4 || 46 || 3.2.5 || &lt;html5media&gt;File:KAP3_46_4.mp3&lt;/html5media&gt;</v>
@@ -35595,6 +35661,9 @@
         <f>VLOOKUP(K47,Side_til_Sektion!A$2:C$217,3,FALSE)</f>
         <v>3.2.9</v>
       </c>
+      <c r="N47" t="s">
+        <v>2343</v>
+      </c>
       <c r="P47" t="str">
         <f t="shared" si="0"/>
         <v>| KAP3_47 || Kapitel || 3 ||  || 47 || 3.2.9 || &lt;html5media&gt;File:KAP3_47.mp3&lt;/html5media&gt;</v>
@@ -35635,6 +35704,9 @@
         <f>VLOOKUP(K48,Side_til_Sektion!A$2:C$217,3,FALSE)</f>
         <v>3.2.9</v>
       </c>
+      <c r="N48" t="s">
+        <v>2343</v>
+      </c>
       <c r="P48" t="str">
         <f t="shared" si="0"/>
         <v>| KAP3_47_2 || Kapitel || 3 || 2 || 47 || 3.2.9 || &lt;html5media&gt;File:KAP3_47_2.mp3&lt;/html5media&gt;</v>
@@ -35675,6 +35747,9 @@
         <f>VLOOKUP(K49,Side_til_Sektion!A$2:C$217,3,FALSE)</f>
         <v>3.2.9</v>
       </c>
+      <c r="N49" t="s">
+        <v>2343</v>
+      </c>
       <c r="P49" t="str">
         <f t="shared" si="0"/>
         <v>| KAP3_47_3 || Kapitel || 3 || 3 || 47 || 3.2.9 || &lt;html5media&gt;File:KAP3_47_3.mp3&lt;/html5media&gt;</v>
@@ -35712,6 +35787,9 @@
         <f>VLOOKUP(K50,Side_til_Sektion!A$2:C$217,3,FALSE)</f>
         <v>3.2.12</v>
       </c>
+      <c r="N50" t="s">
+        <v>2343</v>
+      </c>
       <c r="P50" t="str">
         <f t="shared" si="0"/>
         <v>| KAP3_48 || Kapitel || 3 ||  || 48 || 3.2.12 || &lt;html5media&gt;File:KAP3_48.mp3&lt;/html5media&gt;</v>
@@ -35752,6 +35830,9 @@
         <f>VLOOKUP(K51,Side_til_Sektion!A$2:C$217,3,FALSE)</f>
         <v>3.2.12</v>
       </c>
+      <c r="N51" t="s">
+        <v>2343</v>
+      </c>
       <c r="P51" t="str">
         <f t="shared" si="0"/>
         <v>| KAP3_48_2 || Kapitel || 3 || 2 || 48 || 3.2.12 || &lt;html5media&gt;File:KAP3_48_2.mp3&lt;/html5media&gt;</v>
@@ -35789,6 +35870,9 @@
         <f>VLOOKUP(K52,Side_til_Sektion!A$2:C$217,3,FALSE)</f>
         <v>3.2.14</v>
       </c>
+      <c r="N52" t="s">
+        <v>2343</v>
+      </c>
       <c r="P52" t="str">
         <f t="shared" si="0"/>
         <v>| KAP3_49 || Kapitel || 3 ||  || 49 || 3.2.14 || &lt;html5media&gt;File:KAP3_49.mp3&lt;/html5media&gt;</v>
@@ -35826,6 +35910,9 @@
         <f>VLOOKUP(K53,Side_til_Sektion!A$2:C$217,3,FALSE)</f>
         <v>3.2.15</v>
       </c>
+      <c r="N53" t="s">
+        <v>2343</v>
+      </c>
       <c r="P53" t="str">
         <f t="shared" si="0"/>
         <v>| KAP3_50 || Kapitel || 3 ||  || 50 || 3.2.15 || &lt;html5media&gt;File:KAP3_50.mp3&lt;/html5media&gt;</v>
@@ -35866,6 +35953,9 @@
         <f>VLOOKUP(K54,Side_til_Sektion!A$2:C$217,3,FALSE)</f>
         <v>3.2.15</v>
       </c>
+      <c r="N54" t="s">
+        <v>2343</v>
+      </c>
       <c r="P54" t="str">
         <f t="shared" si="0"/>
         <v>| KAP3_50_2 || Kapitel || 3 || 2 || 50 || 3.2.15 || &lt;html5media&gt;File:KAP3_50_2.mp3&lt;/html5media&gt;</v>
@@ -35906,6 +35996,9 @@
         <f>VLOOKUP(K55,Side_til_Sektion!A$2:C$217,3,FALSE)</f>
         <v>3.2.15</v>
       </c>
+      <c r="N55" t="s">
+        <v>2343</v>
+      </c>
       <c r="P55" t="str">
         <f t="shared" si="0"/>
         <v>| KAP3_50_3 || Kapitel || 3 || 3 || 50 || 3.2.15 || &lt;html5media&gt;File:KAP3_50_3.mp3&lt;/html5media&gt;</v>
@@ -35943,6 +36036,9 @@
         <f>VLOOKUP(K56,Side_til_Sektion!A$2:C$217,3,FALSE)</f>
         <v>3.2.18</v>
       </c>
+      <c r="N56" t="s">
+        <v>2343</v>
+      </c>
       <c r="P56" t="str">
         <f t="shared" si="0"/>
         <v>| KAP3_51 || Kapitel || 3 ||  || 51 || 3.2.18 || &lt;html5media&gt;File:KAP3_51.mp3&lt;/html5media&gt;</v>
@@ -35983,6 +36079,9 @@
         <f>VLOOKUP(K57,Side_til_Sektion!A$2:C$217,3,FALSE)</f>
         <v>3.2.18</v>
       </c>
+      <c r="N57" t="s">
+        <v>2343</v>
+      </c>
       <c r="P57" t="str">
         <f t="shared" si="0"/>
         <v>| KAP3_51_2 || Kapitel || 3 || 2 || 51 || 3.2.18 || &lt;html5media&gt;File:KAP3_51_2.mp3&lt;/html5media&gt;</v>
@@ -36020,6 +36119,9 @@
         <f>VLOOKUP(K58,Side_til_Sektion!A$2:C$217,3,FALSE)</f>
         <v>3.2.20</v>
       </c>
+      <c r="N58" t="s">
+        <v>2343</v>
+      </c>
       <c r="P58" t="str">
         <f t="shared" si="0"/>
         <v>| KAP3_52 || Kapitel || 3 ||  || 52 || 3.2.20 || &lt;html5media&gt;File:KAP3_52.mp3&lt;/html5media&gt;</v>
@@ -36057,6 +36159,9 @@
         <f>VLOOKUP(K59,Side_til_Sektion!A$2:C$217,3,FALSE)</f>
         <v>3.2.21</v>
       </c>
+      <c r="N59" t="s">
+        <v>2343</v>
+      </c>
       <c r="P59" t="str">
         <f t="shared" si="0"/>
         <v>| KAP3_53 || Kapitel || 3 ||  || 53 || 3.2.21 || &lt;html5media&gt;File:KAP3_53.mp3&lt;/html5media&gt;</v>
@@ -36097,6 +36202,9 @@
         <f>VLOOKUP(K60,Side_til_Sektion!A$2:C$217,3,FALSE)</f>
         <v>3.2.21</v>
       </c>
+      <c r="N60" t="s">
+        <v>2343</v>
+      </c>
       <c r="P60" t="str">
         <f t="shared" si="0"/>
         <v>| KAP3_53_2 || Kapitel || 3 || 2 || 53 || 3.2.21 || &lt;html5media&gt;File:KAP3_53_2.mp3&lt;/html5media&gt;</v>
@@ -36134,6 +36242,9 @@
         <f>VLOOKUP(K61,Side_til_Sektion!A$2:C$217,3,FALSE)</f>
         <v>3.4</v>
       </c>
+      <c r="N61" t="s">
+        <v>2343</v>
+      </c>
       <c r="P61" t="str">
         <f t="shared" si="0"/>
         <v>| KAP3_54 || Kapitel || 3 ||  || 54 || 3.4 || &lt;html5media&gt;File:KAP3_54.mp3&lt;/html5media&gt;</v>
@@ -36174,6 +36285,9 @@
         <f>VLOOKUP(K62,Side_til_Sektion!A$2:C$217,3,FALSE)</f>
         <v>3.4</v>
       </c>
+      <c r="N62" t="s">
+        <v>2343</v>
+      </c>
       <c r="P62" t="str">
         <f t="shared" si="0"/>
         <v>| KAP3_54_2 || Kapitel || 3 || 2 || 54 || 3.4 || &lt;html5media&gt;File:KAP3_54_2.mp3&lt;/html5media&gt;</v>
@@ -36211,6 +36325,9 @@
         <f>VLOOKUP(K63,Side_til_Sektion!A$2:C$217,3,FALSE)</f>
         <v>3.4.2</v>
       </c>
+      <c r="N63" t="s">
+        <v>2343</v>
+      </c>
       <c r="P63" t="str">
         <f t="shared" si="0"/>
         <v>| KAP3_56 || Kapitel || 3 ||  || 56 || 3.4.2 || &lt;html5media&gt;File:KAP3_56.mp3&lt;/html5media&gt;</v>
@@ -42684,6 +42801,9 @@
         <f>VLOOKUP(K233,Side_til_Sektion!A$2:C$217,3,FALSE)</f>
         <v>3</v>
       </c>
+      <c r="N233" t="s">
+        <v>2343</v>
+      </c>
       <c r="P233" t="str">
         <f t="shared" si="3"/>
         <v>| BOKS32 || Bokse ||  ||  || 32 || 3 || &lt;html5media&gt;File:BOKS32.mp3&lt;/html5media&gt;</v>
@@ -42718,6 +42838,9 @@
         <f>VLOOKUP(K234,Side_til_Sektion!A$2:C$217,3,FALSE)</f>
         <v>3.1.7</v>
       </c>
+      <c r="N234" t="s">
+        <v>2343</v>
+      </c>
       <c r="P234" t="str">
         <f t="shared" si="3"/>
         <v>| BOKS37 || Bokse ||  ||  || 37 || 3.1.7 || &lt;html5media&gt;File:BOKS37.mp3&lt;/html5media&gt;</v>
@@ -42752,6 +42875,9 @@
         <f>VLOOKUP(K235,Side_til_Sektion!A$2:C$217,3,FALSE)</f>
         <v>3.1.8</v>
       </c>
+      <c r="N235" t="s">
+        <v>2343</v>
+      </c>
       <c r="P235" t="str">
         <f t="shared" si="3"/>
         <v>| BOKS39 || Bokse ||  ||  || 39 || 3.1.8 || &lt;html5media&gt;File:BOKS39.mp3&lt;/html5media&gt;</v>
@@ -42785,6 +42911,9 @@
       <c r="L236" s="7" t="str">
         <f>VLOOKUP(K236,Side_til_Sektion!A$2:C$217,3,FALSE)</f>
         <v>3.2.1</v>
+      </c>
+      <c r="N236" t="s">
+        <v>2343</v>
       </c>
       <c r="P236" t="str">
         <f t="shared" si="3"/>

</xml_diff>